<commit_message>
Se actualiza parte grafica de los vouchers
</commit_message>
<xml_diff>
--- a/teleamiguis/src/main/java/services/banco.xlsx
+++ b/teleamiguis/src/main/java/services/banco.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>NumVoucher</t>
   </si>
@@ -24,9 +24,6 @@
   </si>
   <si>
     <t>Banco</t>
-  </si>
-  <si>
-    <t>Bancolombia</t>
   </si>
   <si>
     <t>Banco de bogota</t>
@@ -80,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -105,10 +102,10 @@
         <v>0.0</v>
       </c>
       <c r="B2" t="n">
-        <v>2533.0</v>
+        <v>2872.0</v>
       </c>
       <c r="C2" t="n">
-        <v>34586.0</v>
+        <v>24120.0</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -119,83 +116,13 @@
         <v>1.0</v>
       </c>
       <c r="B3" t="n">
-        <v>2543.0</v>
+        <v>2871.0</v>
       </c>
       <c r="C3" t="n">
-        <v>7097.0</v>
+        <v>54770.0</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2541.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>54360.0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2542.0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>7838.0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2547.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>40370.0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2545.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>55049.0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2546.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>15125.0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>